<commit_message>
Update to correspond to performance changes in pymassspec and clean up
</commit_message>
<xml_diff>
--- a/UserLibrary.xlsx
+++ b/UserLibrary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ryan\University of Calgary\STRIDE - Minerva - Minerva\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\source\repos\gcms-minerva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{715B73C9-B64E-4020-941F-3E348A2983D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086A103F-E778-4C3E-87C0-D3486B7F0740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="8475" windowWidth="23085" windowHeight="7920"/>
+    <workbookView xWindow="420" yWindow="8475" windowWidth="23085" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLibrary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Source Sheet Order</t>
   </si>
@@ -79,49 +79,10 @@
     <t>inchikey</t>
   </si>
   <si>
-    <t>RI non-polar</t>
-  </si>
-  <si>
-    <t>RI polar</t>
-  </si>
-  <si>
     <t>mw</t>
   </si>
   <si>
     <t>cas#</t>
-  </si>
-  <si>
-    <t>quality</t>
-  </si>
-  <si>
-    <t>odor</t>
-  </si>
-  <si>
-    <t>synonyms</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Conversion Notes</t>
-  </si>
-  <si>
-    <t>DB-5</t>
-  </si>
-  <si>
-    <t>FFAP</t>
-  </si>
-  <si>
-    <t>bLCP</t>
-  </si>
-  <si>
-    <t>aLCP</t>
-  </si>
-  <si>
-    <t>Synonyms</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
   <si>
     <t>BACKGR</t>
@@ -196,7 +157,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1030,10 +991,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1042,7 +1005,7 @@
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,61 +1063,19 @@
       <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="E2" t="s">
         <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
       </c>
       <c r="F2">
         <v>280</v>
@@ -1163,7 +1084,7 @@
         <v>1.5</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>44</v>
@@ -1177,6 +1098,9 @@
       <c r="L2">
         <v>10</v>
       </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
       <c r="Q2">
         <v>43.989829239000002</v>
       </c>
@@ -1184,21 +1108,21 @@
         <v>0.9</v>
       </c>
       <c r="S2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="U2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>977</v>
@@ -1207,7 +1131,7 @@
         <v>1.63</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I3">
         <v>32</v>
@@ -1221,8 +1145,11 @@
       <c r="L3">
         <v>40</v>
       </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="Q3">
         <v>31.989829238999999</v>
@@ -1231,21 +1158,21 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="S3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>14014</v>
@@ -1272,27 +1199,27 @@
         <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q4">
         <v>92.029356027999995</v>
       </c>
       <c r="S4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="T4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="U4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>10913</v>
@@ -1319,19 +1246,19 @@
         <v>640</v>
       </c>
       <c r="P5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="Q5">
         <v>370.09395673</v>
       </c>
       <c r="S5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="U5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>